<commit_message>
update kalk pregled prod 1
</commit_message>
<xml_diff>
--- a/kalk_pregled_prod_1.xlsx
+++ b/kalk_pregled_prod_1.xlsx
@@ -72,7 +72,7 @@
     <t xml:space="preserve">${osnovna_cijena}</t>
   </si>
   <si>
-    <t xml:space="preserve">Ctrl + shift + F9 (rekalkulacija)</t>
+    <t xml:space="preserve">Ctrl + SHIFT + F9 (rekalkulacija)</t>
   </si>
   <si>
     <t xml:space="preserve">cijena</t>
@@ -541,7 +541,7 @@
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>